<commit_message>
Update prompt_experiments_Daily Energy Expenditure through the Human Life Course2023-04-07_1618.xlsx
</commit_message>
<xml_diff>
--- a/output/prompt_experiments_Daily Energy Expenditure through the Human Life Course2023-04-07_1618.xlsx
+++ b/output/prompt_experiments_Daily Energy Expenditure through the Human Life Course2023-04-07_1618.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93345f1c83a5c894/lighthouse/Ginkgo coding/content-summarization/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C618170E-8446-4C1B-96C0-5455D18AD4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{C618170E-8446-4C1B-96C0-5455D18AD4FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFBC9F3A-04B5-49BE-8256-33C598550CC2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prompt_experiments_Daily Energy" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -220,7 +233,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1060,14 +1073,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1416,6 +1429,18 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:XFD1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>